<commit_message>
ausarbeitung und alles sentiment
</commit_message>
<xml_diff>
--- a/Documentation/böhmermannliste Kopie.xlsx
+++ b/Documentation/böhmermannliste Kopie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lisa/Desktop/Seminar/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982804CB-FDB0-504B-A519-EA0F9BC44D40}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D4A9D4-0931-584B-99E7-D145382ABC5A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="460" windowWidth="27840" windowHeight="16600" xr2:uid="{FC8150D4-3350-9642-8667-88427C15149C}"/>
+    <workbookView xWindow="2340" yWindow="1900" windowWidth="27840" windowHeight="16600" xr2:uid="{FC8150D4-3350-9642-8667-88427C15149C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -22843,8 +22843,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:V1456"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1153" workbookViewId="0">
-      <selection activeCell="K1031" sqref="K1031:K1185"/>
+    <sheetView tabSelected="1" topLeftCell="F1013" workbookViewId="0">
+      <selection activeCell="M1025" sqref="M1025"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>